<commit_message>
Update Marcelo report with new repasse rules
</commit_message>
<xml_diff>
--- a/relatorio_marcelo.xlsx
+++ b/relatorio_marcelo.xlsx
@@ -581,11 +581,11 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L2" s="3" t="n">
-        <v>30.0181665</v>
+        <v>0</v>
       </c>
       <c r="M2" t="n">
         <v>3</v>
@@ -634,11 +634,11 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L3" s="3" t="n">
-        <v>40.941219</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
         <v>3</v>
@@ -687,11 +687,11 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L4" s="3" t="n">
-        <v>40.941219</v>
+        <v>0</v>
       </c>
       <c r="M4" t="n">
         <v>3</v>
@@ -740,11 +740,11 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L5" s="3" t="n">
-        <v>37.415181</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
         <v>3</v>
@@ -793,11 +793,11 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L6" s="3" t="n">
-        <v>37.415181</v>
+        <v>0</v>
       </c>
       <c r="M6" t="n">
         <v>3</v>
@@ -846,11 +846,11 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L7" s="3" t="n">
-        <v>28.0251885</v>
+        <v>0</v>
       </c>
       <c r="M7" t="n">
         <v>3</v>
@@ -899,11 +899,11 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L8" s="3" t="n">
-        <v>28.0251885</v>
+        <v>0</v>
       </c>
       <c r="M8" t="n">
         <v>3</v>
@@ -952,11 +952,11 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L9" s="3" t="n">
-        <v>28.0251885</v>
+        <v>0</v>
       </c>
       <c r="M9" t="n">
         <v>3</v>
@@ -1005,11 +1005,11 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L10" s="3" t="n">
-        <v>37.594038</v>
+        <v>0</v>
       </c>
       <c r="M10" t="n">
         <v>3</v>
@@ -1058,11 +1058,11 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L11" s="3" t="n">
-        <v>35.6734545</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
         <v>3</v>
@@ -1111,11 +1111,11 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L12" s="3" t="n">
-        <v>35.68623</v>
+        <v>0</v>
       </c>
       <c r="M12" t="n">
         <v>3</v>
@@ -1164,11 +1164,11 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L13" s="3" t="n">
-        <v>32.083539</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
         <v>3</v>
@@ -1217,11 +1217,11 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L14" s="3" t="n">
-        <v>32.083539</v>
+        <v>0</v>
       </c>
       <c r="M14" t="n">
         <v>3</v>
@@ -1270,11 +1270,11 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L15" s="3" t="n">
-        <v>32.083539</v>
+        <v>0</v>
       </c>
       <c r="M15" t="n">
         <v>3</v>
@@ -1323,11 +1323,11 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L16" s="3" t="n">
-        <v>30.2907105</v>
+        <v>0</v>
       </c>
       <c r="M16" t="n">
         <v>3</v>
@@ -1376,11 +1376,11 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L17" s="3" t="n">
-        <v>30.2907105</v>
+        <v>0</v>
       </c>
       <c r="M17" t="n">
         <v>3</v>
@@ -1429,11 +1429,11 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L18" s="3" t="n">
-        <v>30.2907105</v>
+        <v>0</v>
       </c>
       <c r="M18" t="n">
         <v>3</v>
@@ -1482,11 +1482,11 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L19" s="3" t="n">
-        <v>38.164677</v>
+        <v>0</v>
       </c>
       <c r="M19" t="n">
         <v>3</v>
@@ -1535,11 +1535,11 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L20" s="3" t="n">
-        <v>38.164677</v>
+        <v>0</v>
       </c>
       <c r="M20" t="n">
         <v>3</v>
@@ -1588,11 +1588,11 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L21" s="3" t="n">
-        <v>28.148685</v>
+        <v>0</v>
       </c>
       <c r="M21" t="n">
         <v>3</v>
@@ -1641,11 +1641,11 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L22" s="3" t="n">
-        <v>28.148685</v>
+        <v>0</v>
       </c>
       <c r="M22" t="n">
         <v>3</v>
@@ -1694,11 +1694,11 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L23" s="3" t="n">
-        <v>28.148685</v>
+        <v>0</v>
       </c>
       <c r="M23" t="n">
         <v>3</v>
@@ -1747,11 +1747,11 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L24" s="3" t="n">
-        <v>58.9333815</v>
+        <v>0</v>
       </c>
       <c r="M24" t="n">
         <v>3</v>
@@ -1800,11 +1800,11 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L25" s="3" t="n">
-        <v>58.9333815</v>
+        <v>0</v>
       </c>
       <c r="M25" t="n">
         <v>3</v>
@@ -1853,11 +1853,11 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L26" s="3" t="n">
-        <v>24.639681</v>
+        <v>0</v>
       </c>
       <c r="M26" t="n">
         <v>3</v>
@@ -1906,11 +1906,11 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L27" s="3" t="n">
-        <v>24.639681</v>
+        <v>0</v>
       </c>
       <c r="M27" t="n">
         <v>3</v>
@@ -1959,11 +1959,11 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L28" s="3" t="n">
-        <v>24.639681</v>
+        <v>0</v>
       </c>
       <c r="M28" t="n">
         <v>3</v>
@@ -2012,11 +2012,11 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L29" s="3" t="n">
-        <v>16.6038915</v>
+        <v>0</v>
       </c>
       <c r="M29" t="n">
         <v>3</v>
@@ -2065,11 +2065,11 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L30" s="3" t="n">
-        <v>16.6038915</v>
+        <v>0</v>
       </c>
       <c r="M30" t="n">
         <v>3</v>
@@ -2118,11 +2118,11 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L31" s="3" t="n">
-        <v>16.6038915</v>
+        <v>0</v>
       </c>
       <c r="M31" t="n">
         <v>3</v>
@@ -2171,11 +2171,11 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L32" s="3" t="n">
-        <v>24.5672865</v>
+        <v>0</v>
       </c>
       <c r="M32" t="n">
         <v>3</v>
@@ -2224,11 +2224,11 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L33" s="3" t="n">
-        <v>24.5672865</v>
+        <v>0</v>
       </c>
       <c r="M33" t="n">
         <v>3</v>
@@ -2277,11 +2277,11 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L34" s="3" t="n">
-        <v>24.5672865</v>
+        <v>0</v>
       </c>
       <c r="M34" t="n">
         <v>3</v>
@@ -2330,11 +2330,11 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L35" s="3" t="n">
-        <v>14.3894715</v>
+        <v>0</v>
       </c>
       <c r="M35" t="n">
         <v>4</v>
@@ -2383,11 +2383,11 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L36" s="3" t="n">
-        <v>14.3894715</v>
+        <v>0</v>
       </c>
       <c r="M36" t="n">
         <v>4</v>
@@ -2436,11 +2436,11 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L37" s="3" t="n">
-        <v>40.873083</v>
+        <v>0</v>
       </c>
       <c r="M37" t="n">
         <v>4</v>
@@ -2489,11 +2489,11 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L38" s="3" t="n">
-        <v>40.873083</v>
+        <v>0</v>
       </c>
       <c r="M38" t="n">
         <v>4</v>
@@ -2542,11 +2542,11 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L39" s="3" t="n">
-        <v>40.873083</v>
+        <v>0</v>
       </c>
       <c r="M39" t="n">
         <v>4</v>
@@ -2595,11 +2595,11 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L40" s="3" t="n">
-        <v>40.5025935</v>
+        <v>0</v>
       </c>
       <c r="M40" t="n">
         <v>4</v>
@@ -2648,11 +2648,11 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L41" s="3" t="n">
-        <v>41.55870150000001</v>
+        <v>0</v>
       </c>
       <c r="M41" t="n">
         <v>4</v>
@@ -2701,11 +2701,11 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L42" s="3" t="n">
-        <v>35.958774</v>
+        <v>0</v>
       </c>
       <c r="M42" t="n">
         <v>4</v>
@@ -2754,11 +2754,11 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L43" s="3" t="n">
-        <v>35.958774</v>
+        <v>0</v>
       </c>
       <c r="M43" t="n">
         <v>4</v>
@@ -2807,11 +2807,11 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L44" s="3" t="n">
-        <v>35.958774</v>
+        <v>0</v>
       </c>
       <c r="M44" t="n">
         <v>4</v>
@@ -2860,11 +2860,11 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L45" s="3" t="n">
-        <v>27.3608625</v>
+        <v>0</v>
       </c>
       <c r="M45" t="n">
         <v>4</v>
@@ -2913,11 +2913,11 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L46" s="3" t="n">
-        <v>27.3608625</v>
+        <v>0</v>
       </c>
       <c r="M46" t="n">
         <v>4</v>
@@ -2966,11 +2966,11 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L47" s="3" t="n">
-        <v>27.3608625</v>
+        <v>0</v>
       </c>
       <c r="M47" t="n">
         <v>4</v>
@@ -3019,11 +3019,11 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L48" s="3" t="n">
-        <v>37.81548</v>
+        <v>0</v>
       </c>
       <c r="M48" t="n">
         <v>4</v>
@@ -3072,11 +3072,11 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L49" s="3" t="n">
-        <v>37.81548</v>
+        <v>0</v>
       </c>
       <c r="M49" t="n">
         <v>4</v>
@@ -3125,11 +3125,11 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L50" s="3" t="n">
-        <v>37.81548</v>
+        <v>0</v>
       </c>
       <c r="M50" t="n">
         <v>4</v>
@@ -3178,11 +3178,11 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L51" s="3" t="n">
-        <v>18.8438625</v>
+        <v>0</v>
       </c>
       <c r="M51" t="n">
         <v>4</v>
@@ -3231,11 +3231,11 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L52" s="3" t="n">
-        <v>18.8438625</v>
+        <v>0</v>
       </c>
       <c r="M52" t="n">
         <v>4</v>
@@ -3284,11 +3284,11 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L53" s="3" t="n">
-        <v>18.8438625</v>
+        <v>0</v>
       </c>
       <c r="M53" t="n">
         <v>4</v>
@@ -3337,11 +3337,11 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L54" s="3" t="n">
-        <v>21.9355335</v>
+        <v>0</v>
       </c>
       <c r="M54" t="n">
         <v>4</v>
@@ -3390,11 +3390,11 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L55" s="3" t="n">
-        <v>21.9355335</v>
+        <v>0</v>
       </c>
       <c r="M55" t="n">
         <v>4</v>
@@ -3443,11 +3443,11 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L56" s="3" t="n">
-        <v>21.9355335</v>
+        <v>0</v>
       </c>
       <c r="M56" t="n">
         <v>4</v>
@@ -3496,11 +3496,11 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L57" s="3" t="n">
-        <v>42.2485785</v>
+        <v>0</v>
       </c>
       <c r="M57" t="n">
         <v>4</v>
@@ -3549,11 +3549,11 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L58" s="3" t="n">
-        <v>42.2485785</v>
+        <v>0</v>
       </c>
       <c r="M58" t="n">
         <v>4</v>
@@ -3602,11 +3602,11 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L59" s="3" t="n">
-        <v>42.2485785</v>
+        <v>0</v>
       </c>
       <c r="M59" t="n">
         <v>4</v>
@@ -3655,7 +3655,7 @@
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L60" s="3" t="n">
@@ -3708,7 +3708,7 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L61" s="3" t="n">
@@ -3761,11 +3761,11 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L62" s="3" t="n">
-        <v>23.651709</v>
+        <v>0</v>
       </c>
       <c r="M62" t="n">
         <v>11</v>
@@ -3814,11 +3814,11 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L63" s="3" t="n">
-        <v>22.9746075</v>
+        <v>0</v>
       </c>
       <c r="M63" t="n">
         <v>13</v>
@@ -3867,11 +3867,11 @@
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L64" s="3" t="n">
-        <v>146.8799235</v>
+        <v>0</v>
       </c>
       <c r="M64" t="n">
         <v>14</v>
@@ -3920,11 +3920,11 @@
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L65" s="3" t="n">
-        <v>169.5095925</v>
+        <v>0</v>
       </c>
       <c r="M65" t="n">
         <v>14</v>
@@ -3973,11 +3973,11 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L66" s="3" t="n">
-        <v>139.346637</v>
+        <v>0</v>
       </c>
       <c r="M66" t="n">
         <v>14</v>
@@ -4026,11 +4026,11 @@
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L67" s="3" t="n">
-        <v>140.027997</v>
+        <v>0</v>
       </c>
       <c r="M67" t="n">
         <v>14</v>
@@ -4079,11 +4079,11 @@
       </c>
       <c r="K68" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L68" s="3" t="n">
-        <v>12.69033</v>
+        <v>0</v>
       </c>
       <c r="M68" t="n">
         <v>14</v>
@@ -4132,11 +4132,11 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L69" s="3" t="n">
-        <v>148.0297185</v>
+        <v>0</v>
       </c>
       <c r="M69" t="n">
         <v>14</v>
@@ -4185,7 +4185,7 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L70" s="3" t="n">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L71" s="3" t="n">
@@ -4291,7 +4291,7 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L72" s="3" t="n">
@@ -4344,7 +4344,7 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L73" s="3" t="n">
@@ -4397,7 +4397,7 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L74" s="3" t="n">
@@ -4450,7 +4450,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L75" s="3" t="n">
@@ -4503,7 +4503,7 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L76" s="3" t="n">
@@ -4556,7 +4556,7 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L77" s="3" t="n">
@@ -4609,7 +4609,7 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L78" s="3" t="n">
@@ -4662,7 +4662,7 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L79" s="3" t="n">
@@ -4715,7 +4715,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L80" s="3" t="n">
@@ -4768,7 +4768,7 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L81" s="3" t="n">
@@ -4821,7 +4821,7 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L82" s="3" t="n">
@@ -4874,7 +4874,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L83" s="3" t="n">
@@ -4927,7 +4927,7 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L84" s="3" t="n">
@@ -4980,7 +4980,7 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L85" s="3" t="n">
@@ -5033,7 +5033,7 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L86" s="3" t="n">
@@ -5086,7 +5086,7 @@
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L87" s="3" t="n">
@@ -5139,7 +5139,7 @@
       </c>
       <c r="K88" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L88" s="3" t="n">
@@ -5192,7 +5192,7 @@
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L89" s="3" t="n">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="K90" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L90" s="3" t="n">
@@ -5298,7 +5298,7 @@
       </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L91" s="3" t="n">
@@ -5351,7 +5351,7 @@
       </c>
       <c r="K92" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L92" s="3" t="n">
@@ -5404,7 +5404,7 @@
       </c>
       <c r="K93" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L93" s="3" t="n">
@@ -5457,7 +5457,7 @@
       </c>
       <c r="K94" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L94" s="3" t="n">
@@ -5510,11 +5510,11 @@
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L95" s="3" t="n">
-        <v>17.5577955</v>
+        <v>0</v>
       </c>
       <c r="M95" t="n">
         <v>17</v>
@@ -5563,11 +5563,11 @@
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L96" s="3" t="n">
-        <v>15.9395655</v>
+        <v>0</v>
       </c>
       <c r="M96" t="n">
         <v>17</v>
@@ -5616,11 +5616,11 @@
       </c>
       <c r="K97" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L97" s="3" t="n">
-        <v>17.860149</v>
+        <v>0</v>
       </c>
       <c r="M97" t="n">
         <v>17</v>
@@ -5669,11 +5669,11 @@
       </c>
       <c r="K98" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L98" s="3" t="n">
-        <v>25.346592</v>
+        <v>0</v>
       </c>
       <c r="M98" t="n">
         <v>17</v>
@@ -5722,11 +5722,11 @@
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L99" s="3" t="n">
-        <v>18.2050875</v>
+        <v>0</v>
       </c>
       <c r="M99" t="n">
         <v>17</v>
@@ -5775,11 +5775,11 @@
       </c>
       <c r="K100" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L100" s="3" t="n">
-        <v>51.5832105</v>
+        <v>0</v>
       </c>
       <c r="M100" t="n">
         <v>17</v>
@@ -5828,7 +5828,7 @@
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L101" s="3" t="n">
@@ -5881,7 +5881,7 @@
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L102" s="3" t="n">
@@ -5934,7 +5934,7 @@
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L103" s="3" t="n">
@@ -5987,7 +5987,7 @@
       </c>
       <c r="K104" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L104" s="3" t="n">
@@ -6040,7 +6040,7 @@
       </c>
       <c r="K105" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L105" s="3" t="n">
@@ -6093,7 +6093,7 @@
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L106" s="3" t="n">
@@ -6146,7 +6146,7 @@
       </c>
       <c r="K107" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L107" s="3" t="n">
@@ -6199,7 +6199,7 @@
       </c>
       <c r="K108" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L108" s="3" t="n">
@@ -6252,7 +6252,7 @@
       </c>
       <c r="K109" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L109" s="3" t="n">
@@ -6305,7 +6305,7 @@
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L110" s="3" t="n">
@@ -6358,7 +6358,7 @@
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L111" s="3" t="n">
@@ -6411,7 +6411,7 @@
       </c>
       <c r="K112" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L112" s="3" t="n">
@@ -6464,7 +6464,7 @@
       </c>
       <c r="K113" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L113" s="3" t="n">
@@ -6517,7 +6517,7 @@
       </c>
       <c r="K114" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L114" s="3" t="n">
@@ -6570,7 +6570,7 @@
       </c>
       <c r="K115" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L115" s="3" t="n">
@@ -6623,7 +6623,7 @@
       </c>
       <c r="K116" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L116" s="3" t="n">
@@ -6676,7 +6676,7 @@
       </c>
       <c r="K117" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L117" s="3" t="n">
@@ -6729,7 +6729,7 @@
       </c>
       <c r="K118" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L118" s="3" t="n">
@@ -6782,7 +6782,7 @@
       </c>
       <c r="K119" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L119" s="3" t="n">
@@ -6835,7 +6835,7 @@
       </c>
       <c r="K120" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L120" s="3" t="n">
@@ -6888,7 +6888,7 @@
       </c>
       <c r="K121" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L121" s="3" t="n">
@@ -6941,7 +6941,7 @@
       </c>
       <c r="K122" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L122" s="3" t="n">
@@ -6994,7 +6994,7 @@
       </c>
       <c r="K123" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L123" s="3" t="n">
@@ -7047,7 +7047,7 @@
       </c>
       <c r="K124" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L124" s="3" t="n">
@@ -7100,7 +7100,7 @@
       </c>
       <c r="K125" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L125" s="3" t="n">
@@ -7153,7 +7153,7 @@
       </c>
       <c r="K126" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L126" s="3" t="n">
@@ -7206,7 +7206,7 @@
       </c>
       <c r="K127" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L127" s="3" t="n">
@@ -7259,7 +7259,7 @@
       </c>
       <c r="K128" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L128" s="3" t="n">
@@ -7312,7 +7312,7 @@
       </c>
       <c r="K129" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L129" s="3" t="n">
@@ -7365,7 +7365,7 @@
       </c>
       <c r="K130" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L130" s="3" t="n">
@@ -7418,7 +7418,7 @@
       </c>
       <c r="K131" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L131" s="3" t="n">
@@ -7471,7 +7471,7 @@
       </c>
       <c r="K132" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L132" s="3" t="n">
@@ -7524,7 +7524,7 @@
       </c>
       <c r="K133" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L133" s="3" t="n">
@@ -7577,11 +7577,11 @@
       </c>
       <c r="K134" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L134" s="3" t="n">
-        <v>23.856117</v>
+        <v>0</v>
       </c>
       <c r="M134" t="n">
         <v>21</v>
@@ -7630,11 +7630,11 @@
       </c>
       <c r="K135" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L135" s="3" t="n">
-        <v>36.043944</v>
+        <v>0</v>
       </c>
       <c r="M135" t="n">
         <v>21</v>
@@ -7683,11 +7683,11 @@
       </c>
       <c r="K136" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L136" s="3" t="n">
-        <v>23.225859</v>
+        <v>0</v>
       </c>
       <c r="M136" t="n">
         <v>21</v>
@@ -7736,11 +7736,11 @@
       </c>
       <c r="K137" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L137" s="3" t="n">
-        <v>57.183138</v>
+        <v>0</v>
       </c>
       <c r="M137" t="n">
         <v>27</v>
@@ -7789,11 +7789,11 @@
       </c>
       <c r="K138" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L138" s="3" t="n">
-        <v>23.438784</v>
+        <v>0</v>
       </c>
       <c r="M138" t="n">
         <v>31</v>
@@ -7842,11 +7842,11 @@
       </c>
       <c r="K139" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L139" s="3" t="n">
-        <v>26.930754</v>
+        <v>0</v>
       </c>
       <c r="M139" t="n">
         <v>31</v>
@@ -7895,11 +7895,11 @@
       </c>
       <c r="K140" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L140" s="3" t="n">
-        <v>28.1359095</v>
+        <v>0</v>
       </c>
       <c r="M140" t="n">
         <v>31</v>
@@ -7948,11 +7948,11 @@
       </c>
       <c r="K141" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L141" s="3" t="n">
-        <v>26.8072575</v>
+        <v>0</v>
       </c>
       <c r="M141" t="n">
         <v>31</v>
@@ -8001,11 +8001,11 @@
       </c>
       <c r="K142" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L142" s="3" t="n">
-        <v>32.4455115</v>
+        <v>0</v>
       </c>
       <c r="M142" t="n">
         <v>31</v>
@@ -8054,11 +8054,11 @@
       </c>
       <c r="K143" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L143" s="3" t="n">
-        <v>9.760482000000001</v>
+        <v>0</v>
       </c>
       <c r="M143" t="n">
         <v>31</v>
@@ -8107,11 +8107,11 @@
       </c>
       <c r="K144" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L144" s="3" t="n">
-        <v>12.3028065</v>
+        <v>0</v>
       </c>
       <c r="M144" t="n">
         <v>31</v>
@@ -8160,11 +8160,11 @@
       </c>
       <c r="K145" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L145" s="3" t="n">
-        <v>29.860602</v>
+        <v>0</v>
       </c>
       <c r="M145" t="n">
         <v>32</v>
@@ -8213,11 +8213,11 @@
       </c>
       <c r="K146" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L146" s="3" t="n">
-        <v>4.982444999999999</v>
+        <v>0</v>
       </c>
       <c r="M146" t="n">
         <v>34</v>
@@ -8266,7 +8266,7 @@
       </c>
       <c r="K147" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L147" s="3" t="n">
@@ -8319,7 +8319,7 @@
       </c>
       <c r="K148" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L148" s="3" t="n">
@@ -8372,7 +8372,7 @@
       </c>
       <c r="K149" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L149" s="3" t="n">
@@ -8425,7 +8425,7 @@
       </c>
       <c r="K150" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L150" s="3" t="n">
@@ -8478,7 +8478,7 @@
       </c>
       <c r="K151" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L151" s="3" t="n">
@@ -8531,7 +8531,7 @@
       </c>
       <c r="K152" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L152" s="3" t="n">
@@ -8584,7 +8584,7 @@
       </c>
       <c r="K153" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L153" s="3" t="n">
@@ -8637,7 +8637,7 @@
       </c>
       <c r="K154" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L154" s="3" t="n">
@@ -8690,7 +8690,7 @@
       </c>
       <c r="K155" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L155" s="3" t="n">
@@ -8743,7 +8743,7 @@
       </c>
       <c r="K156" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L156" s="3" t="n">
@@ -8796,7 +8796,7 @@
       </c>
       <c r="K157" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L157" s="3" t="n">
@@ -8849,7 +8849,7 @@
       </c>
       <c r="K158" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L158" s="3" t="n">
@@ -8902,7 +8902,7 @@
       </c>
       <c r="K159" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L159" s="3" t="n">
@@ -8955,11 +8955,11 @@
       </c>
       <c r="K160" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L160" s="3" t="n">
-        <v>33.6208575</v>
+        <v>0</v>
       </c>
       <c r="M160" t="n">
         <v>38</v>
@@ -9008,11 +9008,11 @@
       </c>
       <c r="K161" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L161" s="3" t="n">
-        <v>46.2600855</v>
+        <v>0</v>
       </c>
       <c r="M161" t="n">
         <v>38</v>
@@ -9061,11 +9061,11 @@
       </c>
       <c r="K162" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L162" s="3" t="n">
-        <v>23.4856275</v>
+        <v>0</v>
       </c>
       <c r="M162" t="n">
         <v>38</v>
@@ -9114,11 +9114,11 @@
       </c>
       <c r="K163" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L163" s="3" t="n">
-        <v>24.222348</v>
+        <v>0</v>
       </c>
       <c r="M163" t="n">
         <v>38</v>
@@ -9167,11 +9167,11 @@
       </c>
       <c r="K164" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L164" s="3" t="n">
-        <v>24.7291095</v>
+        <v>0</v>
       </c>
       <c r="M164" t="n">
         <v>38</v>
@@ -9220,11 +9220,11 @@
       </c>
       <c r="K165" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L165" s="3" t="n">
-        <v>26.4410265</v>
+        <v>0</v>
       </c>
       <c r="M165" t="n">
         <v>38</v>
@@ -9273,11 +9273,11 @@
       </c>
       <c r="K166" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L166" s="3" t="n">
-        <v>39.961764</v>
+        <v>0</v>
       </c>
       <c r="M166" t="n">
         <v>38</v>
@@ -9326,11 +9326,11 @@
       </c>
       <c r="K167" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L167" s="3" t="n">
-        <v>18.3072915</v>
+        <v>0</v>
       </c>
       <c r="M167" t="n">
         <v>38</v>
@@ -9379,11 +9379,11 @@
       </c>
       <c r="K168" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L168" s="3" t="n">
-        <v>28.753392</v>
+        <v>0</v>
       </c>
       <c r="M168" t="n">
         <v>38</v>
@@ -9432,11 +9432,11 @@
       </c>
       <c r="K169" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L169" s="3" t="n">
-        <v>31.325526</v>
+        <v>0</v>
       </c>
       <c r="M169" t="n">
         <v>38</v>
@@ -9485,11 +9485,11 @@
       </c>
       <c r="K170" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L170" s="3" t="n">
-        <v>25.917231</v>
+        <v>0</v>
       </c>
       <c r="M170" t="n">
         <v>39</v>
@@ -9538,11 +9538,11 @@
       </c>
       <c r="K171" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L171" s="3" t="n">
-        <v>19.0738215</v>
+        <v>0</v>
       </c>
       <c r="M171" t="n">
         <v>39</v>
@@ -9591,11 +9591,11 @@
       </c>
       <c r="K172" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L172" s="3" t="n">
-        <v>19.0738215</v>
+        <v>0</v>
       </c>
       <c r="M172" t="n">
         <v>39</v>
@@ -9644,11 +9644,11 @@
       </c>
       <c r="K173" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L173" s="3" t="n">
-        <v>25.917231</v>
+        <v>0</v>
       </c>
       <c r="M173" t="n">
         <v>39</v>
@@ -9697,11 +9697,11 @@
       </c>
       <c r="K174" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L174" s="3" t="n">
-        <v>70.23544050000001</v>
+        <v>0</v>
       </c>
       <c r="M174" t="n">
         <v>39</v>
@@ -9750,11 +9750,11 @@
       </c>
       <c r="K175" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L175" s="3" t="n">
-        <v>25.917231</v>
+        <v>0</v>
       </c>
       <c r="M175" t="n">
         <v>39</v>
@@ -9803,7 +9803,7 @@
       </c>
       <c r="K176" t="inlineStr">
         <is>
-          <t>*0,8517*0,2</t>
+          <t>*0,8517*0,1</t>
         </is>
       </c>
       <c r="L176" s="3" t="n">
@@ -9856,11 +9856,11 @@
       </c>
       <c r="K177" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L177" s="3" t="n">
-        <v>9.522005999999999</v>
+        <v>0</v>
       </c>
       <c r="M177" t="n">
         <v>40</v>
@@ -9909,11 +9909,11 @@
       </c>
       <c r="K178" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L178" s="3" t="n">
-        <v>26.8072575</v>
+        <v>0</v>
       </c>
       <c r="M178" t="n">
         <v>40</v>
@@ -9962,11 +9962,11 @@
       </c>
       <c r="K179" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L179" s="3" t="n">
-        <v>31.606587</v>
+        <v>0</v>
       </c>
       <c r="M179" t="n">
         <v>40</v>
@@ -10015,11 +10015,11 @@
       </c>
       <c r="K180" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L180" s="3" t="n">
-        <v>29.255895</v>
+        <v>0</v>
       </c>
       <c r="M180" t="n">
         <v>40</v>
@@ -10068,11 +10068,11 @@
       </c>
       <c r="K181" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L181" s="3" t="n">
-        <v>25.7681835</v>
+        <v>0</v>
       </c>
       <c r="M181" t="n">
         <v>41</v>
@@ -10121,11 +10121,11 @@
       </c>
       <c r="K182" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L182" s="3" t="n">
-        <v>9.9861825</v>
+        <v>0</v>
       </c>
       <c r="M182" t="n">
         <v>41</v>
@@ -10174,11 +10174,11 @@
       </c>
       <c r="K183" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L183" s="3" t="n">
-        <v>48.2530635</v>
+        <v>0</v>
       </c>
       <c r="M183" t="n">
         <v>41</v>
@@ -10227,11 +10227,11 @@
       </c>
       <c r="K184" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L184" s="3" t="n">
-        <v>50.0331165</v>
+        <v>0</v>
       </c>
       <c r="M184" t="n">
         <v>41</v>
@@ -10280,11 +10280,11 @@
       </c>
       <c r="K185" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L185" s="3" t="n">
-        <v>10.331121</v>
+        <v>0</v>
       </c>
       <c r="M185" t="n">
         <v>41</v>
@@ -10333,11 +10333,11 @@
       </c>
       <c r="K186" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L186" s="3" t="n">
-        <v>27.305502</v>
+        <v>0</v>
       </c>
       <c r="M186" t="n">
         <v>41</v>
@@ -10386,11 +10386,11 @@
       </c>
       <c r="K187" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L187" s="3" t="n">
-        <v>10.067094</v>
+        <v>0</v>
       </c>
       <c r="M187" t="n">
         <v>53</v>
@@ -10439,11 +10439,11 @@
       </c>
       <c r="K188" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L188" s="3" t="n">
-        <v>9.411285000000001</v>
+        <v>0</v>
       </c>
       <c r="M188" t="n">
         <v>53</v>
@@ -10492,11 +10492,11 @@
       </c>
       <c r="K189" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L189" s="3" t="n">
-        <v>9.223911000000001</v>
+        <v>0</v>
       </c>
       <c r="M189" t="n">
         <v>53</v>
@@ -10545,11 +10545,11 @@
       </c>
       <c r="K190" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L190" s="3" t="n">
-        <v>27.4545495</v>
+        <v>0</v>
       </c>
       <c r="M190" t="n">
         <v>53</v>
@@ -10598,11 +10598,11 @@
       </c>
       <c r="K191" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L191" s="3" t="n">
-        <v>18.490407</v>
+        <v>0</v>
       </c>
       <c r="M191" t="n">
         <v>58</v>
@@ -10651,11 +10651,11 @@
       </c>
       <c r="K192" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L192" s="3" t="n">
-        <v>29.860602</v>
+        <v>0</v>
       </c>
       <c r="M192" t="n">
         <v>58</v>
@@ -10704,11 +10704,11 @@
       </c>
       <c r="K193" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L193" s="3" t="n">
-        <v>18.532992</v>
+        <v>0</v>
       </c>
       <c r="M193" t="n">
         <v>58</v>
@@ -10757,11 +10757,11 @@
       </c>
       <c r="K194" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L194" s="3" t="n">
-        <v>17.1574965</v>
+        <v>0</v>
       </c>
       <c r="M194" t="n">
         <v>58</v>
@@ -10810,11 +10810,11 @@
       </c>
       <c r="K195" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L195" s="3" t="n">
-        <v>30.013908</v>
+        <v>0</v>
       </c>
       <c r="M195" t="n">
         <v>58</v>
@@ -10863,11 +10863,11 @@
       </c>
       <c r="K196" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L196" s="3" t="n">
-        <v>28.36161</v>
+        <v>0</v>
       </c>
       <c r="M196" t="n">
         <v>58</v>
@@ -10916,11 +10916,11 @@
       </c>
       <c r="K197" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L197" s="3" t="n">
-        <v>28.36161</v>
+        <v>0</v>
       </c>
       <c r="M197" t="n">
         <v>58</v>
@@ -10969,11 +10969,11 @@
       </c>
       <c r="K198" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L198" s="3" t="n">
-        <v>28.36161</v>
+        <v>0</v>
       </c>
       <c r="M198" t="n">
         <v>58</v>
@@ -11022,11 +11022,11 @@
       </c>
       <c r="K199" t="inlineStr">
         <is>
-          <t>*0,8517/2</t>
+          <t>*0,8517*0,25</t>
         </is>
       </c>
       <c r="L199" s="3" t="n">
-        <v>20.815548</v>
+        <v>0</v>
       </c>
       <c r="M199" t="n">
         <v>58</v>
@@ -11109,7 +11109,7 @@
         <v>4543.4</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>1934.80689</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -11147,7 +11147,7 @@
         <v>55.54</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>23.651709</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -11166,7 +11166,7 @@
         <v>53.95</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>22.9746075</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -11185,7 +11185,7 @@
         <v>1776.41</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>756.4841985</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -11223,7 +11223,7 @@
         <v>222.87</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>94.9091895</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -11242,7 +11242,7 @@
         <v>121.13</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>51.5832105</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -11337,7 +11337,7 @@
         <v>56.02</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>23.856117</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -11356,7 +11356,7 @@
         <v>139.18</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>59.269803</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -11375,7 +11375,7 @@
         <v>134.28</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>57.183138</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -11394,7 +11394,7 @@
         <v>323.49</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>137.7582165</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -11413,7 +11413,7 @@
         <v>51.81</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>22.0632885</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -11432,7 +11432,7 @@
         <v>70.12</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>29.860602</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -11451,7 +11451,7 @@
         <v>11.7</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>4.982444999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -11489,7 +11489,7 @@
         <v>697.6800000000001</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>297.107028</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -11508,7 +11508,7 @@
         <v>437.09</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>186.1347765</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -11546,7 +11546,7 @@
         <v>159.53</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>67.9358505</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -11565,7 +11565,7 @@
         <v>152.66</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>65.010261</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -11584,7 +11584,7 @@
         <v>230.8</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>98.28618</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -11603,7 +11603,7 @@
         <v>88.38000000000001</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>37.636623</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -11622,7 +11622,7 @@
         <v>131.87</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>56.1568395</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -11641,7 +11641,7 @@
         <v>43.42</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>18.490407</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -11660,7 +11660,7 @@
         <v>224.41</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>95.5649985</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -11726,7 +11726,7 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>4141.706378999999</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Marcelo totals formulas
</commit_message>
<xml_diff>
--- a/relatorio_marcelo.xlsx
+++ b/relatorio_marcelo.xlsx
@@ -11715,8 +11715,9 @@
           <t>Total Comissão Base</t>
         </is>
       </c>
-      <c r="B2" s="3" t="n">
-        <v>17319.31</v>
+      <c r="B2" s="3">
+        <f>SUM('Transações'!J2:J199)</f>
+        <v/>
       </c>
     </row>
     <row r="3">
@@ -11725,8 +11726,9 @@
           <t>Total Comissão Vendedor</t>
         </is>
       </c>
-      <c r="B3" s="3" t="n">
-        <v>0</v>
+      <c r="B3" s="3">
+        <f>SUM('Transações'!L2:L199)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Marcelo vendor commission calc
</commit_message>
<xml_diff>
--- a/relatorio_marcelo.xlsx
+++ b/relatorio_marcelo.xlsx
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="L2" s="3" t="n">
-        <v>0</v>
+        <v>15.00908325</v>
       </c>
       <c r="M2" t="n">
         <v>3</v>
@@ -638,7 +638,7 @@
         </is>
       </c>
       <c r="L3" s="3" t="n">
-        <v>0</v>
+        <v>20.4706095</v>
       </c>
       <c r="M3" t="n">
         <v>3</v>
@@ -691,7 +691,7 @@
         </is>
       </c>
       <c r="L4" s="3" t="n">
-        <v>0</v>
+        <v>20.4706095</v>
       </c>
       <c r="M4" t="n">
         <v>3</v>
@@ -744,7 +744,7 @@
         </is>
       </c>
       <c r="L5" s="3" t="n">
-        <v>0</v>
+        <v>18.7075905</v>
       </c>
       <c r="M5" t="n">
         <v>3</v>
@@ -797,7 +797,7 @@
         </is>
       </c>
       <c r="L6" s="3" t="n">
-        <v>0</v>
+        <v>18.7075905</v>
       </c>
       <c r="M6" t="n">
         <v>3</v>
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="L7" s="3" t="n">
-        <v>0</v>
+        <v>14.01259425</v>
       </c>
       <c r="M7" t="n">
         <v>3</v>
@@ -903,7 +903,7 @@
         </is>
       </c>
       <c r="L8" s="3" t="n">
-        <v>0</v>
+        <v>14.01259425</v>
       </c>
       <c r="M8" t="n">
         <v>3</v>
@@ -956,7 +956,7 @@
         </is>
       </c>
       <c r="L9" s="3" t="n">
-        <v>0</v>
+        <v>14.01259425</v>
       </c>
       <c r="M9" t="n">
         <v>3</v>
@@ -1009,7 +1009,7 @@
         </is>
       </c>
       <c r="L10" s="3" t="n">
-        <v>0</v>
+        <v>18.797019</v>
       </c>
       <c r="M10" t="n">
         <v>3</v>
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="L11" s="3" t="n">
-        <v>0</v>
+        <v>17.83672725</v>
       </c>
       <c r="M11" t="n">
         <v>3</v>
@@ -1115,7 +1115,7 @@
         </is>
       </c>
       <c r="L12" s="3" t="n">
-        <v>0</v>
+        <v>17.843115</v>
       </c>
       <c r="M12" t="n">
         <v>3</v>
@@ -1168,7 +1168,7 @@
         </is>
       </c>
       <c r="L13" s="3" t="n">
-        <v>0</v>
+        <v>16.0417695</v>
       </c>
       <c r="M13" t="n">
         <v>3</v>
@@ -1221,7 +1221,7 @@
         </is>
       </c>
       <c r="L14" s="3" t="n">
-        <v>0</v>
+        <v>16.0417695</v>
       </c>
       <c r="M14" t="n">
         <v>3</v>
@@ -1274,7 +1274,7 @@
         </is>
       </c>
       <c r="L15" s="3" t="n">
-        <v>0</v>
+        <v>16.0417695</v>
       </c>
       <c r="M15" t="n">
         <v>3</v>
@@ -1327,7 +1327,7 @@
         </is>
       </c>
       <c r="L16" s="3" t="n">
-        <v>0</v>
+        <v>15.14535525</v>
       </c>
       <c r="M16" t="n">
         <v>3</v>
@@ -1380,7 +1380,7 @@
         </is>
       </c>
       <c r="L17" s="3" t="n">
-        <v>0</v>
+        <v>15.14535525</v>
       </c>
       <c r="M17" t="n">
         <v>3</v>
@@ -1433,7 +1433,7 @@
         </is>
       </c>
       <c r="L18" s="3" t="n">
-        <v>0</v>
+        <v>15.14535525</v>
       </c>
       <c r="M18" t="n">
         <v>3</v>
@@ -1486,7 +1486,7 @@
         </is>
       </c>
       <c r="L19" s="3" t="n">
-        <v>0</v>
+        <v>19.0823385</v>
       </c>
       <c r="M19" t="n">
         <v>3</v>
@@ -1539,7 +1539,7 @@
         </is>
       </c>
       <c r="L20" s="3" t="n">
-        <v>0</v>
+        <v>19.0823385</v>
       </c>
       <c r="M20" t="n">
         <v>3</v>
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="L21" s="3" t="n">
-        <v>0</v>
+        <v>14.0743425</v>
       </c>
       <c r="M21" t="n">
         <v>3</v>
@@ -1645,7 +1645,7 @@
         </is>
       </c>
       <c r="L22" s="3" t="n">
-        <v>0</v>
+        <v>14.0743425</v>
       </c>
       <c r="M22" t="n">
         <v>3</v>
@@ -1698,7 +1698,7 @@
         </is>
       </c>
       <c r="L23" s="3" t="n">
-        <v>0</v>
+        <v>14.0743425</v>
       </c>
       <c r="M23" t="n">
         <v>3</v>
@@ -1751,7 +1751,7 @@
         </is>
       </c>
       <c r="L24" s="3" t="n">
-        <v>0</v>
+        <v>29.46669075</v>
       </c>
       <c r="M24" t="n">
         <v>3</v>
@@ -1804,7 +1804,7 @@
         </is>
       </c>
       <c r="L25" s="3" t="n">
-        <v>0</v>
+        <v>29.46669075</v>
       </c>
       <c r="M25" t="n">
         <v>3</v>
@@ -1857,7 +1857,7 @@
         </is>
       </c>
       <c r="L26" s="3" t="n">
-        <v>0</v>
+        <v>12.3198405</v>
       </c>
       <c r="M26" t="n">
         <v>3</v>
@@ -1910,7 +1910,7 @@
         </is>
       </c>
       <c r="L27" s="3" t="n">
-        <v>0</v>
+        <v>12.3198405</v>
       </c>
       <c r="M27" t="n">
         <v>3</v>
@@ -1963,7 +1963,7 @@
         </is>
       </c>
       <c r="L28" s="3" t="n">
-        <v>0</v>
+        <v>12.3198405</v>
       </c>
       <c r="M28" t="n">
         <v>3</v>
@@ -2016,7 +2016,7 @@
         </is>
       </c>
       <c r="L29" s="3" t="n">
-        <v>0</v>
+        <v>8.30194575</v>
       </c>
       <c r="M29" t="n">
         <v>3</v>
@@ -2069,7 +2069,7 @@
         </is>
       </c>
       <c r="L30" s="3" t="n">
-        <v>0</v>
+        <v>8.30194575</v>
       </c>
       <c r="M30" t="n">
         <v>3</v>
@@ -2122,7 +2122,7 @@
         </is>
       </c>
       <c r="L31" s="3" t="n">
-        <v>0</v>
+        <v>8.30194575</v>
       </c>
       <c r="M31" t="n">
         <v>3</v>
@@ -2175,7 +2175,7 @@
         </is>
       </c>
       <c r="L32" s="3" t="n">
-        <v>0</v>
+        <v>12.28364325</v>
       </c>
       <c r="M32" t="n">
         <v>3</v>
@@ -2228,7 +2228,7 @@
         </is>
       </c>
       <c r="L33" s="3" t="n">
-        <v>0</v>
+        <v>12.28364325</v>
       </c>
       <c r="M33" t="n">
         <v>3</v>
@@ -2281,7 +2281,7 @@
         </is>
       </c>
       <c r="L34" s="3" t="n">
-        <v>0</v>
+        <v>12.28364325</v>
       </c>
       <c r="M34" t="n">
         <v>3</v>
@@ -2334,7 +2334,7 @@
         </is>
       </c>
       <c r="L35" s="3" t="n">
-        <v>0</v>
+        <v>7.19473575</v>
       </c>
       <c r="M35" t="n">
         <v>4</v>
@@ -2387,7 +2387,7 @@
         </is>
       </c>
       <c r="L36" s="3" t="n">
-        <v>0</v>
+        <v>7.19473575</v>
       </c>
       <c r="M36" t="n">
         <v>4</v>
@@ -2440,7 +2440,7 @@
         </is>
       </c>
       <c r="L37" s="3" t="n">
-        <v>0</v>
+        <v>20.4365415</v>
       </c>
       <c r="M37" t="n">
         <v>4</v>
@@ -2493,7 +2493,7 @@
         </is>
       </c>
       <c r="L38" s="3" t="n">
-        <v>0</v>
+        <v>20.4365415</v>
       </c>
       <c r="M38" t="n">
         <v>4</v>
@@ -2546,7 +2546,7 @@
         </is>
       </c>
       <c r="L39" s="3" t="n">
-        <v>0</v>
+        <v>20.4365415</v>
       </c>
       <c r="M39" t="n">
         <v>4</v>
@@ -2599,7 +2599,7 @@
         </is>
       </c>
       <c r="L40" s="3" t="n">
-        <v>0</v>
+        <v>20.25129675</v>
       </c>
       <c r="M40" t="n">
         <v>4</v>
@@ -2652,7 +2652,7 @@
         </is>
       </c>
       <c r="L41" s="3" t="n">
-        <v>0</v>
+        <v>20.77935075</v>
       </c>
       <c r="M41" t="n">
         <v>4</v>
@@ -2705,7 +2705,7 @@
         </is>
       </c>
       <c r="L42" s="3" t="n">
-        <v>0</v>
+        <v>17.979387</v>
       </c>
       <c r="M42" t="n">
         <v>4</v>
@@ -2758,7 +2758,7 @@
         </is>
       </c>
       <c r="L43" s="3" t="n">
-        <v>0</v>
+        <v>17.979387</v>
       </c>
       <c r="M43" t="n">
         <v>4</v>
@@ -2811,7 +2811,7 @@
         </is>
       </c>
       <c r="L44" s="3" t="n">
-        <v>0</v>
+        <v>17.979387</v>
       </c>
       <c r="M44" t="n">
         <v>4</v>
@@ -2864,7 +2864,7 @@
         </is>
       </c>
       <c r="L45" s="3" t="n">
-        <v>0</v>
+        <v>13.68043125</v>
       </c>
       <c r="M45" t="n">
         <v>4</v>
@@ -2917,7 +2917,7 @@
         </is>
       </c>
       <c r="L46" s="3" t="n">
-        <v>0</v>
+        <v>13.68043125</v>
       </c>
       <c r="M46" t="n">
         <v>4</v>
@@ -2970,7 +2970,7 @@
         </is>
       </c>
       <c r="L47" s="3" t="n">
-        <v>0</v>
+        <v>13.68043125</v>
       </c>
       <c r="M47" t="n">
         <v>4</v>
@@ -3023,7 +3023,7 @@
         </is>
       </c>
       <c r="L48" s="3" t="n">
-        <v>0</v>
+        <v>18.90774</v>
       </c>
       <c r="M48" t="n">
         <v>4</v>
@@ -3076,7 +3076,7 @@
         </is>
       </c>
       <c r="L49" s="3" t="n">
-        <v>0</v>
+        <v>18.90774</v>
       </c>
       <c r="M49" t="n">
         <v>4</v>
@@ -3129,7 +3129,7 @@
         </is>
       </c>
       <c r="L50" s="3" t="n">
-        <v>0</v>
+        <v>18.90774</v>
       </c>
       <c r="M50" t="n">
         <v>4</v>
@@ -3182,7 +3182,7 @@
         </is>
       </c>
       <c r="L51" s="3" t="n">
-        <v>0</v>
+        <v>9.42193125</v>
       </c>
       <c r="M51" t="n">
         <v>4</v>
@@ -3235,7 +3235,7 @@
         </is>
       </c>
       <c r="L52" s="3" t="n">
-        <v>0</v>
+        <v>9.42193125</v>
       </c>
       <c r="M52" t="n">
         <v>4</v>
@@ -3288,7 +3288,7 @@
         </is>
       </c>
       <c r="L53" s="3" t="n">
-        <v>0</v>
+        <v>9.42193125</v>
       </c>
       <c r="M53" t="n">
         <v>4</v>
@@ -3341,7 +3341,7 @@
         </is>
       </c>
       <c r="L54" s="3" t="n">
-        <v>0</v>
+        <v>10.96776675</v>
       </c>
       <c r="M54" t="n">
         <v>4</v>
@@ -3394,7 +3394,7 @@
         </is>
       </c>
       <c r="L55" s="3" t="n">
-        <v>0</v>
+        <v>10.96776675</v>
       </c>
       <c r="M55" t="n">
         <v>4</v>
@@ -3447,7 +3447,7 @@
         </is>
       </c>
       <c r="L56" s="3" t="n">
-        <v>0</v>
+        <v>10.96776675</v>
       </c>
       <c r="M56" t="n">
         <v>4</v>
@@ -3500,7 +3500,7 @@
         </is>
       </c>
       <c r="L57" s="3" t="n">
-        <v>0</v>
+        <v>21.12428925</v>
       </c>
       <c r="M57" t="n">
         <v>4</v>
@@ -3553,7 +3553,7 @@
         </is>
       </c>
       <c r="L58" s="3" t="n">
-        <v>0</v>
+        <v>21.12428925</v>
       </c>
       <c r="M58" t="n">
         <v>4</v>
@@ -3606,7 +3606,7 @@
         </is>
       </c>
       <c r="L59" s="3" t="n">
-        <v>0</v>
+        <v>21.12428925</v>
       </c>
       <c r="M59" t="n">
         <v>4</v>
@@ -3659,7 +3659,7 @@
         </is>
       </c>
       <c r="L60" s="3" t="n">
-        <v>0</v>
+        <v>4.777185300000001</v>
       </c>
       <c r="M60" t="n">
         <v>11</v>
@@ -3712,7 +3712,7 @@
         </is>
       </c>
       <c r="L61" s="3" t="n">
-        <v>0</v>
+        <v>6.879180900000001</v>
       </c>
       <c r="M61" t="n">
         <v>11</v>
@@ -3765,7 +3765,7 @@
         </is>
       </c>
       <c r="L62" s="3" t="n">
-        <v>0</v>
+        <v>11.8258545</v>
       </c>
       <c r="M62" t="n">
         <v>11</v>
@@ -3818,7 +3818,7 @@
         </is>
       </c>
       <c r="L63" s="3" t="n">
-        <v>0</v>
+        <v>11.48730375</v>
       </c>
       <c r="M63" t="n">
         <v>13</v>
@@ -3871,7 +3871,7 @@
         </is>
       </c>
       <c r="L64" s="3" t="n">
-        <v>0</v>
+        <v>73.43996175000001</v>
       </c>
       <c r="M64" t="n">
         <v>14</v>
@@ -3924,7 +3924,7 @@
         </is>
       </c>
       <c r="L65" s="3" t="n">
-        <v>0</v>
+        <v>84.75479625</v>
       </c>
       <c r="M65" t="n">
         <v>14</v>
@@ -3977,7 +3977,7 @@
         </is>
       </c>
       <c r="L66" s="3" t="n">
-        <v>0</v>
+        <v>69.67331850000001</v>
       </c>
       <c r="M66" t="n">
         <v>14</v>
@@ -4030,7 +4030,7 @@
         </is>
       </c>
       <c r="L67" s="3" t="n">
-        <v>0</v>
+        <v>70.0139985</v>
       </c>
       <c r="M67" t="n">
         <v>14</v>
@@ -4083,7 +4083,7 @@
         </is>
       </c>
       <c r="L68" s="3" t="n">
-        <v>0</v>
+        <v>6.345165000000001</v>
       </c>
       <c r="M68" t="n">
         <v>14</v>
@@ -4136,7 +4136,7 @@
         </is>
       </c>
       <c r="L69" s="3" t="n">
-        <v>0</v>
+        <v>74.01485925</v>
       </c>
       <c r="M69" t="n">
         <v>14</v>
@@ -4189,7 +4189,7 @@
         </is>
       </c>
       <c r="L70" s="3" t="n">
-        <v>0</v>
+        <v>4.9960722</v>
       </c>
       <c r="M70" t="n">
         <v>16</v>
@@ -4242,7 +4242,7 @@
         </is>
       </c>
       <c r="L71" s="3" t="n">
-        <v>0</v>
+        <v>5.364006600000001</v>
       </c>
       <c r="M71" t="n">
         <v>16</v>
@@ -4295,7 +4295,7 @@
         </is>
       </c>
       <c r="L72" s="3" t="n">
-        <v>0</v>
+        <v>5.333345400000001</v>
       </c>
       <c r="M72" t="n">
         <v>16</v>
@@ -4348,7 +4348,7 @@
         </is>
       </c>
       <c r="L73" s="3" t="n">
-        <v>0</v>
+        <v>4.936453200000001</v>
       </c>
       <c r="M73" t="n">
         <v>16</v>
@@ -4401,7 +4401,7 @@
         </is>
       </c>
       <c r="L74" s="3" t="n">
-        <v>0</v>
+        <v>5.048877600000001</v>
       </c>
       <c r="M74" t="n">
         <v>16</v>
@@ -4454,7 +4454,7 @@
         </is>
       </c>
       <c r="L75" s="3" t="n">
-        <v>0</v>
+        <v>5.297574000000001</v>
       </c>
       <c r="M75" t="n">
         <v>16</v>
@@ -4507,7 +4507,7 @@
         </is>
       </c>
       <c r="L76" s="3" t="n">
-        <v>0</v>
+        <v>5.6663601</v>
       </c>
       <c r="M76" t="n">
         <v>16</v>
@@ -4560,7 +4560,7 @@
         </is>
       </c>
       <c r="L77" s="3" t="n">
-        <v>0</v>
+        <v>5.725127400000001</v>
       </c>
       <c r="M77" t="n">
         <v>16</v>
@@ -4613,7 +4613,7 @@
         </is>
       </c>
       <c r="L78" s="3" t="n">
-        <v>0</v>
+        <v>4.943266800000001</v>
       </c>
       <c r="M78" t="n">
         <v>16</v>
@@ -4666,7 +4666,7 @@
         </is>
       </c>
       <c r="L79" s="3" t="n">
-        <v>0</v>
+        <v>4.800181200000001</v>
       </c>
       <c r="M79" t="n">
         <v>16</v>
@@ -4719,7 +4719,7 @@
         </is>
       </c>
       <c r="L80" s="3" t="n">
-        <v>0</v>
+        <v>4.8708723</v>
       </c>
       <c r="M80" t="n">
         <v>16</v>
@@ -4772,7 +4772,7 @@
         </is>
       </c>
       <c r="L81" s="3" t="n">
-        <v>0</v>
+        <v>4.8521349</v>
       </c>
       <c r="M81" t="n">
         <v>16</v>
@@ -4825,7 +4825,7 @@
         </is>
       </c>
       <c r="L82" s="3" t="n">
-        <v>0</v>
+        <v>5.699576400000001</v>
       </c>
       <c r="M82" t="n">
         <v>16</v>
@@ -4878,7 +4878,7 @@
         </is>
       </c>
       <c r="L83" s="3" t="n">
-        <v>0</v>
+        <v>4.7601513</v>
       </c>
       <c r="M83" t="n">
         <v>16</v>
@@ -4931,7 +4931,7 @@
         </is>
       </c>
       <c r="L84" s="3" t="n">
-        <v>0</v>
+        <v>4.4066958</v>
       </c>
       <c r="M84" t="n">
         <v>16</v>
@@ -4984,7 +4984,7 @@
         </is>
       </c>
       <c r="L85" s="3" t="n">
-        <v>0</v>
+        <v>5.427032400000001</v>
       </c>
       <c r="M85" t="n">
         <v>16</v>
@@ -5037,7 +5037,7 @@
         </is>
       </c>
       <c r="L86" s="3" t="n">
-        <v>0</v>
+        <v>4.962855900000001</v>
       </c>
       <c r="M86" t="n">
         <v>16</v>
@@ -5090,7 +5090,7 @@
         </is>
       </c>
       <c r="L87" s="3" t="n">
-        <v>0</v>
+        <v>4.7473758</v>
       </c>
       <c r="M87" t="n">
         <v>16</v>
@@ -5143,7 +5143,7 @@
         </is>
       </c>
       <c r="L88" s="3" t="n">
-        <v>0</v>
+        <v>4.712456100000001</v>
       </c>
       <c r="M88" t="n">
         <v>16</v>
@@ -5196,7 +5196,7 @@
         </is>
       </c>
       <c r="L89" s="3" t="n">
-        <v>0</v>
+        <v>5.003737500000001</v>
       </c>
       <c r="M89" t="n">
         <v>16</v>
@@ -5249,7 +5249,7 @@
         </is>
       </c>
       <c r="L90" s="3" t="n">
-        <v>0</v>
+        <v>4.632396300000001</v>
       </c>
       <c r="M90" t="n">
         <v>16</v>
@@ -5302,7 +5302,7 @@
         </is>
       </c>
       <c r="L91" s="3" t="n">
-        <v>0</v>
+        <v>4.93986</v>
       </c>
       <c r="M91" t="n">
         <v>16</v>
@@ -5355,7 +5355,7 @@
         </is>
       </c>
       <c r="L92" s="3" t="n">
-        <v>0</v>
+        <v>5.565007800000001</v>
       </c>
       <c r="M92" t="n">
         <v>16</v>
@@ -5408,7 +5408,7 @@
         </is>
       </c>
       <c r="L93" s="3" t="n">
-        <v>0</v>
+        <v>4.707345900000001</v>
       </c>
       <c r="M93" t="n">
         <v>16</v>
@@ -5461,7 +5461,7 @@
         </is>
       </c>
       <c r="L94" s="3" t="n">
-        <v>0</v>
+        <v>4.8759825</v>
       </c>
       <c r="M94" t="n">
         <v>16</v>
@@ -5514,7 +5514,7 @@
         </is>
       </c>
       <c r="L95" s="3" t="n">
-        <v>0</v>
+        <v>8.778897749999999</v>
       </c>
       <c r="M95" t="n">
         <v>17</v>
@@ -5567,7 +5567,7 @@
         </is>
       </c>
       <c r="L96" s="3" t="n">
-        <v>0</v>
+        <v>7.96978275</v>
       </c>
       <c r="M96" t="n">
         <v>17</v>
@@ -5620,7 +5620,7 @@
         </is>
       </c>
       <c r="L97" s="3" t="n">
-        <v>0</v>
+        <v>8.9300745</v>
       </c>
       <c r="M97" t="n">
         <v>17</v>
@@ -5673,7 +5673,7 @@
         </is>
       </c>
       <c r="L98" s="3" t="n">
-        <v>0</v>
+        <v>12.673296</v>
       </c>
       <c r="M98" t="n">
         <v>17</v>
@@ -5726,7 +5726,7 @@
         </is>
       </c>
       <c r="L99" s="3" t="n">
-        <v>0</v>
+        <v>9.102543750000001</v>
       </c>
       <c r="M99" t="n">
         <v>17</v>
@@ -5779,7 +5779,7 @@
         </is>
       </c>
       <c r="L100" s="3" t="n">
-        <v>0</v>
+        <v>25.79160525</v>
       </c>
       <c r="M100" t="n">
         <v>17</v>
@@ -5832,7 +5832,7 @@
         </is>
       </c>
       <c r="L101" s="3" t="n">
-        <v>0</v>
+        <v>16.9198722</v>
       </c>
       <c r="M101" t="n">
         <v>20</v>
@@ -5885,7 +5885,7 @@
         </is>
       </c>
       <c r="L102" s="3" t="n">
-        <v>0</v>
+        <v>9.051015900000001</v>
       </c>
       <c r="M102" t="n">
         <v>20</v>
@@ -5938,7 +5938,7 @@
         </is>
       </c>
       <c r="L103" s="3" t="n">
-        <v>0</v>
+        <v>24.9181869</v>
       </c>
       <c r="M103" t="n">
         <v>20</v>
@@ -5991,7 +5991,7 @@
         </is>
       </c>
       <c r="L104" s="3" t="n">
-        <v>0</v>
+        <v>11.0474007</v>
       </c>
       <c r="M104" t="n">
         <v>20</v>
@@ -6044,7 +6044,7 @@
         </is>
       </c>
       <c r="L105" s="3" t="n">
-        <v>0</v>
+        <v>33.92746950000001</v>
       </c>
       <c r="M105" t="n">
         <v>20</v>
@@ -6097,7 +6097,7 @@
         </is>
       </c>
       <c r="L106" s="3" t="n">
-        <v>0</v>
+        <v>24.7597707</v>
       </c>
       <c r="M106" t="n">
         <v>20</v>
@@ -6150,7 +6150,7 @@
         </is>
       </c>
       <c r="L107" s="3" t="n">
-        <v>0</v>
+        <v>24.7597707</v>
       </c>
       <c r="M107" t="n">
         <v>20</v>
@@ -6203,7 +6203,7 @@
         </is>
       </c>
       <c r="L108" s="3" t="n">
-        <v>0</v>
+        <v>2.8881147</v>
       </c>
       <c r="M108" t="n">
         <v>20</v>
@@ -6256,7 +6256,7 @@
         </is>
       </c>
       <c r="L109" s="3" t="n">
-        <v>0</v>
+        <v>2.8881147</v>
       </c>
       <c r="M109" t="n">
         <v>20</v>
@@ -6309,7 +6309,7 @@
         </is>
       </c>
       <c r="L110" s="3" t="n">
-        <v>0</v>
+        <v>2.8974834</v>
       </c>
       <c r="M110" t="n">
         <v>20</v>
@@ -6362,7 +6362,7 @@
         </is>
       </c>
       <c r="L111" s="3" t="n">
-        <v>0</v>
+        <v>8.565546900000001</v>
       </c>
       <c r="M111" t="n">
         <v>20</v>
@@ -6415,7 +6415,7 @@
         </is>
       </c>
       <c r="L112" s="3" t="n">
-        <v>0</v>
+        <v>8.565546900000001</v>
       </c>
       <c r="M112" t="n">
         <v>20</v>
@@ -6468,7 +6468,7 @@
         </is>
       </c>
       <c r="L113" s="3" t="n">
-        <v>0</v>
+        <v>2.9954289</v>
       </c>
       <c r="M113" t="n">
         <v>20</v>
@@ -6521,7 +6521,7 @@
         </is>
       </c>
       <c r="L114" s="3" t="n">
-        <v>0</v>
+        <v>3.0047976</v>
       </c>
       <c r="M114" t="n">
         <v>20</v>
@@ -6574,7 +6574,7 @@
         </is>
       </c>
       <c r="L115" s="3" t="n">
-        <v>0</v>
+        <v>3.0925227</v>
       </c>
       <c r="M115" t="n">
         <v>20</v>
@@ -6627,7 +6627,7 @@
         </is>
       </c>
       <c r="L116" s="3" t="n">
-        <v>0</v>
+        <v>3.1018914</v>
       </c>
       <c r="M116" t="n">
         <v>20</v>
@@ -6680,7 +6680,7 @@
         </is>
       </c>
       <c r="L117" s="3" t="n">
-        <v>0</v>
+        <v>2.8710807</v>
       </c>
       <c r="M117" t="n">
         <v>20</v>
@@ -6733,7 +6733,7 @@
         </is>
       </c>
       <c r="L118" s="3" t="n">
-        <v>0</v>
+        <v>2.8710807</v>
       </c>
       <c r="M118" t="n">
         <v>20</v>
@@ -6786,7 +6786,7 @@
         </is>
       </c>
       <c r="L119" s="3" t="n">
-        <v>0</v>
+        <v>2.879597700000001</v>
       </c>
       <c r="M119" t="n">
         <v>20</v>
@@ -6839,7 +6839,7 @@
         </is>
       </c>
       <c r="L120" s="3" t="n">
-        <v>0</v>
+        <v>2.9715813</v>
       </c>
       <c r="M120" t="n">
         <v>20</v>
@@ -6892,7 +6892,7 @@
         </is>
       </c>
       <c r="L121" s="3" t="n">
-        <v>0</v>
+        <v>2.9715813</v>
       </c>
       <c r="M121" t="n">
         <v>20</v>
@@ -6945,7 +6945,7 @@
         </is>
       </c>
       <c r="L122" s="3" t="n">
-        <v>0</v>
+        <v>3.4894149</v>
       </c>
       <c r="M122" t="n">
         <v>20</v>
@@ -6998,7 +6998,7 @@
         </is>
       </c>
       <c r="L123" s="3" t="n">
-        <v>0</v>
+        <v>5.943162600000001</v>
       </c>
       <c r="M123" t="n">
         <v>20</v>
@@ -7051,7 +7051,7 @@
         </is>
       </c>
       <c r="L124" s="3" t="n">
-        <v>0</v>
+        <v>5.9610483</v>
       </c>
       <c r="M124" t="n">
         <v>20</v>
@@ -7104,7 +7104,7 @@
         </is>
       </c>
       <c r="L125" s="3" t="n">
-        <v>0</v>
+        <v>9.024613200000001</v>
       </c>
       <c r="M125" t="n">
         <v>20</v>
@@ -7157,7 +7157,7 @@
         </is>
       </c>
       <c r="L126" s="3" t="n">
-        <v>0</v>
+        <v>9.024613200000001</v>
       </c>
       <c r="M126" t="n">
         <v>20</v>
@@ -7210,7 +7210,7 @@
         </is>
       </c>
       <c r="L127" s="3" t="n">
-        <v>0</v>
+        <v>9.051867600000001</v>
       </c>
       <c r="M127" t="n">
         <v>21</v>
@@ -7263,7 +7263,7 @@
         </is>
       </c>
       <c r="L128" s="3" t="n">
-        <v>0</v>
+        <v>6.1083924</v>
       </c>
       <c r="M128" t="n">
         <v>21</v>
@@ -7316,7 +7316,7 @@
         </is>
       </c>
       <c r="L129" s="3" t="n">
-        <v>0</v>
+        <v>6.1083924</v>
       </c>
       <c r="M129" t="n">
         <v>21</v>
@@ -7369,7 +7369,7 @@
         </is>
       </c>
       <c r="L130" s="3" t="n">
-        <v>0</v>
+        <v>6.127129800000001</v>
       </c>
       <c r="M130" t="n">
         <v>21</v>
@@ -7422,7 +7422,7 @@
         </is>
       </c>
       <c r="L131" s="3" t="n">
-        <v>0</v>
+        <v>12.0796611</v>
       </c>
       <c r="M131" t="n">
         <v>21</v>
@@ -7475,7 +7475,7 @@
         </is>
       </c>
       <c r="L132" s="3" t="n">
-        <v>0</v>
+        <v>12.0796611</v>
       </c>
       <c r="M132" t="n">
         <v>21</v>
@@ -7528,7 +7528,7 @@
         </is>
       </c>
       <c r="L133" s="3" t="n">
-        <v>0</v>
+        <v>12.1154325</v>
       </c>
       <c r="M133" t="n">
         <v>21</v>
@@ -7581,7 +7581,7 @@
         </is>
       </c>
       <c r="L134" s="3" t="n">
-        <v>0</v>
+        <v>11.9280585</v>
       </c>
       <c r="M134" t="n">
         <v>21</v>
@@ -7634,7 +7634,7 @@
         </is>
       </c>
       <c r="L135" s="3" t="n">
-        <v>0</v>
+        <v>18.021972</v>
       </c>
       <c r="M135" t="n">
         <v>21</v>
@@ -7687,7 +7687,7 @@
         </is>
       </c>
       <c r="L136" s="3" t="n">
-        <v>0</v>
+        <v>11.6129295</v>
       </c>
       <c r="M136" t="n">
         <v>21</v>
@@ -7740,7 +7740,7 @@
         </is>
       </c>
       <c r="L137" s="3" t="n">
-        <v>0</v>
+        <v>28.591569</v>
       </c>
       <c r="M137" t="n">
         <v>27</v>
@@ -7793,7 +7793,7 @@
         </is>
       </c>
       <c r="L138" s="3" t="n">
-        <v>0</v>
+        <v>11.719392</v>
       </c>
       <c r="M138" t="n">
         <v>31</v>
@@ -7846,7 +7846,7 @@
         </is>
       </c>
       <c r="L139" s="3" t="n">
-        <v>0</v>
+        <v>13.465377</v>
       </c>
       <c r="M139" t="n">
         <v>31</v>
@@ -7899,7 +7899,7 @@
         </is>
       </c>
       <c r="L140" s="3" t="n">
-        <v>0</v>
+        <v>14.06795475</v>
       </c>
       <c r="M140" t="n">
         <v>31</v>
@@ -7952,7 +7952,7 @@
         </is>
       </c>
       <c r="L141" s="3" t="n">
-        <v>0</v>
+        <v>13.40362875</v>
       </c>
       <c r="M141" t="n">
         <v>31</v>
@@ -8005,7 +8005,7 @@
         </is>
       </c>
       <c r="L142" s="3" t="n">
-        <v>0</v>
+        <v>16.22275575</v>
       </c>
       <c r="M142" t="n">
         <v>31</v>
@@ -8058,7 +8058,7 @@
         </is>
       </c>
       <c r="L143" s="3" t="n">
-        <v>0</v>
+        <v>4.880241000000001</v>
       </c>
       <c r="M143" t="n">
         <v>31</v>
@@ -8111,7 +8111,7 @@
         </is>
       </c>
       <c r="L144" s="3" t="n">
-        <v>0</v>
+        <v>6.15140325</v>
       </c>
       <c r="M144" t="n">
         <v>31</v>
@@ -8164,7 +8164,7 @@
         </is>
       </c>
       <c r="L145" s="3" t="n">
-        <v>0</v>
+        <v>14.930301</v>
       </c>
       <c r="M145" t="n">
         <v>32</v>
@@ -8217,7 +8217,7 @@
         </is>
       </c>
       <c r="L146" s="3" t="n">
-        <v>0</v>
+        <v>2.4912225</v>
       </c>
       <c r="M146" t="n">
         <v>34</v>
@@ -8270,7 +8270,7 @@
         </is>
       </c>
       <c r="L147" s="3" t="n">
-        <v>0</v>
+        <v>11.5243527</v>
       </c>
       <c r="M147" t="n">
         <v>34</v>
@@ -8323,7 +8323,7 @@
         </is>
       </c>
       <c r="L148" s="3" t="n">
-        <v>0</v>
+        <v>11.3250549</v>
       </c>
       <c r="M148" t="n">
         <v>34</v>
@@ -8376,7 +8376,7 @@
         </is>
       </c>
       <c r="L149" s="3" t="n">
-        <v>0</v>
+        <v>11.549052</v>
       </c>
       <c r="M149" t="n">
         <v>34</v>
@@ -8429,7 +8429,7 @@
         </is>
       </c>
       <c r="L150" s="3" t="n">
-        <v>0</v>
+        <v>11.4289623</v>
       </c>
       <c r="M150" t="n">
         <v>34</v>
@@ -8482,7 +8482,7 @@
         </is>
       </c>
       <c r="L151" s="3" t="n">
-        <v>0</v>
+        <v>12.528507</v>
       </c>
       <c r="M151" t="n">
         <v>34</v>
@@ -8535,7 +8535,7 @@
         </is>
       </c>
       <c r="L152" s="3" t="n">
-        <v>0</v>
+        <v>11.5558656</v>
       </c>
       <c r="M152" t="n">
         <v>34</v>
@@ -8588,7 +8588,7 @@
         </is>
       </c>
       <c r="L153" s="3" t="n">
-        <v>0</v>
+        <v>3.815616</v>
       </c>
       <c r="M153" t="n">
         <v>34</v>
@@ -8641,7 +8641,7 @@
         </is>
       </c>
       <c r="L154" s="3" t="n">
-        <v>0</v>
+        <v>11.2279611</v>
       </c>
       <c r="M154" t="n">
         <v>34</v>
@@ -8694,7 +8694,7 @@
         </is>
       </c>
       <c r="L155" s="3" t="n">
-        <v>0</v>
+        <v>18.9102951</v>
       </c>
       <c r="M155" t="n">
         <v>34</v>
@@ -8747,7 +8747,7 @@
         </is>
       </c>
       <c r="L156" s="3" t="n">
-        <v>0</v>
+        <v>30.8920107</v>
       </c>
       <c r="M156" t="n">
         <v>34</v>
@@ -8800,7 +8800,7 @@
         </is>
       </c>
       <c r="L157" s="3" t="n">
-        <v>0</v>
+        <v>12.9603189</v>
       </c>
       <c r="M157" t="n">
         <v>34</v>
@@ -8853,7 +8853,7 @@
         </is>
       </c>
       <c r="L158" s="3" t="n">
-        <v>0</v>
+        <v>30.8332434</v>
       </c>
       <c r="M158" t="n">
         <v>34</v>
@@ -8906,7 +8906,7 @@
         </is>
       </c>
       <c r="L159" s="3" t="n">
-        <v>0</v>
+        <v>22.8988062</v>
       </c>
       <c r="M159" t="n">
         <v>34</v>
@@ -8959,7 +8959,7 @@
         </is>
       </c>
       <c r="L160" s="3" t="n">
-        <v>0</v>
+        <v>16.81042875</v>
       </c>
       <c r="M160" t="n">
         <v>38</v>
@@ -9012,7 +9012,7 @@
         </is>
       </c>
       <c r="L161" s="3" t="n">
-        <v>0</v>
+        <v>23.13004275</v>
       </c>
       <c r="M161" t="n">
         <v>38</v>
@@ -9065,7 +9065,7 @@
         </is>
       </c>
       <c r="L162" s="3" t="n">
-        <v>0</v>
+        <v>11.74281375</v>
       </c>
       <c r="M162" t="n">
         <v>38</v>
@@ -9118,7 +9118,7 @@
         </is>
       </c>
       <c r="L163" s="3" t="n">
-        <v>0</v>
+        <v>12.111174</v>
       </c>
       <c r="M163" t="n">
         <v>38</v>
@@ -9171,7 +9171,7 @@
         </is>
       </c>
       <c r="L164" s="3" t="n">
-        <v>0</v>
+        <v>12.36455475</v>
       </c>
       <c r="M164" t="n">
         <v>38</v>
@@ -9224,7 +9224,7 @@
         </is>
       </c>
       <c r="L165" s="3" t="n">
-        <v>0</v>
+        <v>13.22051325</v>
       </c>
       <c r="M165" t="n">
         <v>38</v>
@@ -9277,7 +9277,7 @@
         </is>
       </c>
       <c r="L166" s="3" t="n">
-        <v>0</v>
+        <v>19.980882</v>
       </c>
       <c r="M166" t="n">
         <v>38</v>
@@ -9330,7 +9330,7 @@
         </is>
       </c>
       <c r="L167" s="3" t="n">
-        <v>0</v>
+        <v>9.153645750000001</v>
       </c>
       <c r="M167" t="n">
         <v>38</v>
@@ -9383,7 +9383,7 @@
         </is>
       </c>
       <c r="L168" s="3" t="n">
-        <v>0</v>
+        <v>14.376696</v>
       </c>
       <c r="M168" t="n">
         <v>38</v>
@@ -9436,7 +9436,7 @@
         </is>
       </c>
       <c r="L169" s="3" t="n">
-        <v>0</v>
+        <v>15.662763</v>
       </c>
       <c r="M169" t="n">
         <v>38</v>
@@ -9489,7 +9489,7 @@
         </is>
       </c>
       <c r="L170" s="3" t="n">
-        <v>0</v>
+        <v>12.9586155</v>
       </c>
       <c r="M170" t="n">
         <v>39</v>
@@ -9542,7 +9542,7 @@
         </is>
       </c>
       <c r="L171" s="3" t="n">
-        <v>0</v>
+        <v>9.536910750000001</v>
       </c>
       <c r="M171" t="n">
         <v>39</v>
@@ -9595,7 +9595,7 @@
         </is>
       </c>
       <c r="L172" s="3" t="n">
-        <v>0</v>
+        <v>9.536910750000001</v>
       </c>
       <c r="M172" t="n">
         <v>39</v>
@@ -9648,7 +9648,7 @@
         </is>
       </c>
       <c r="L173" s="3" t="n">
-        <v>0</v>
+        <v>12.9586155</v>
       </c>
       <c r="M173" t="n">
         <v>39</v>
@@ -9701,7 +9701,7 @@
         </is>
       </c>
       <c r="L174" s="3" t="n">
-        <v>0</v>
+        <v>35.11772025</v>
       </c>
       <c r="M174" t="n">
         <v>39</v>
@@ -9754,7 +9754,7 @@
         </is>
       </c>
       <c r="L175" s="3" t="n">
-        <v>0</v>
+        <v>12.9586155</v>
       </c>
       <c r="M175" t="n">
         <v>39</v>
@@ -9807,7 +9807,7 @@
         </is>
       </c>
       <c r="L176" s="3" t="n">
-        <v>0</v>
+        <v>12.3019548</v>
       </c>
       <c r="M176" t="n">
         <v>39</v>
@@ -9860,7 +9860,7 @@
         </is>
       </c>
       <c r="L177" s="3" t="n">
-        <v>0</v>
+        <v>4.761003</v>
       </c>
       <c r="M177" t="n">
         <v>40</v>
@@ -9913,7 +9913,7 @@
         </is>
       </c>
       <c r="L178" s="3" t="n">
-        <v>0</v>
+        <v>13.40362875</v>
       </c>
       <c r="M178" t="n">
         <v>40</v>
@@ -9966,7 +9966,7 @@
         </is>
       </c>
       <c r="L179" s="3" t="n">
-        <v>0</v>
+        <v>15.8032935</v>
       </c>
       <c r="M179" t="n">
         <v>40</v>
@@ -10019,7 +10019,7 @@
         </is>
       </c>
       <c r="L180" s="3" t="n">
-        <v>0</v>
+        <v>14.6279475</v>
       </c>
       <c r="M180" t="n">
         <v>40</v>
@@ -10072,7 +10072,7 @@
         </is>
       </c>
       <c r="L181" s="3" t="n">
-        <v>0</v>
+        <v>12.88409175</v>
       </c>
       <c r="M181" t="n">
         <v>41</v>
@@ -10125,7 +10125,7 @@
         </is>
       </c>
       <c r="L182" s="3" t="n">
-        <v>0</v>
+        <v>4.99309125</v>
       </c>
       <c r="M182" t="n">
         <v>41</v>
@@ -10178,7 +10178,7 @@
         </is>
       </c>
       <c r="L183" s="3" t="n">
-        <v>0</v>
+        <v>24.12653175</v>
       </c>
       <c r="M183" t="n">
         <v>41</v>
@@ -10231,7 +10231,7 @@
         </is>
       </c>
       <c r="L184" s="3" t="n">
-        <v>0</v>
+        <v>25.01655825</v>
       </c>
       <c r="M184" t="n">
         <v>41</v>
@@ -10284,7 +10284,7 @@
         </is>
       </c>
       <c r="L185" s="3" t="n">
-        <v>0</v>
+        <v>5.165560500000001</v>
       </c>
       <c r="M185" t="n">
         <v>41</v>
@@ -10337,7 +10337,7 @@
         </is>
       </c>
       <c r="L186" s="3" t="n">
-        <v>0</v>
+        <v>13.652751</v>
       </c>
       <c r="M186" t="n">
         <v>41</v>
@@ -10390,7 +10390,7 @@
         </is>
       </c>
       <c r="L187" s="3" t="n">
-        <v>0</v>
+        <v>5.033547</v>
       </c>
       <c r="M187" t="n">
         <v>53</v>
@@ -10443,7 +10443,7 @@
         </is>
       </c>
       <c r="L188" s="3" t="n">
-        <v>0</v>
+        <v>4.705642500000001</v>
       </c>
       <c r="M188" t="n">
         <v>53</v>
@@ -10496,7 +10496,7 @@
         </is>
       </c>
       <c r="L189" s="3" t="n">
-        <v>0</v>
+        <v>4.611955500000001</v>
       </c>
       <c r="M189" t="n">
         <v>53</v>
@@ -10549,7 +10549,7 @@
         </is>
       </c>
       <c r="L190" s="3" t="n">
-        <v>0</v>
+        <v>13.72727475</v>
       </c>
       <c r="M190" t="n">
         <v>53</v>
@@ -10602,7 +10602,7 @@
         </is>
       </c>
       <c r="L191" s="3" t="n">
-        <v>0</v>
+        <v>9.245203500000001</v>
       </c>
       <c r="M191" t="n">
         <v>58</v>
@@ -10655,7 +10655,7 @@
         </is>
       </c>
       <c r="L192" s="3" t="n">
-        <v>0</v>
+        <v>14.930301</v>
       </c>
       <c r="M192" t="n">
         <v>58</v>
@@ -10708,7 +10708,7 @@
         </is>
       </c>
       <c r="L193" s="3" t="n">
-        <v>0</v>
+        <v>9.266496</v>
       </c>
       <c r="M193" t="n">
         <v>58</v>
@@ -10761,7 +10761,7 @@
         </is>
       </c>
       <c r="L194" s="3" t="n">
-        <v>0</v>
+        <v>8.57874825</v>
       </c>
       <c r="M194" t="n">
         <v>58</v>
@@ -10814,7 +10814,7 @@
         </is>
       </c>
       <c r="L195" s="3" t="n">
-        <v>0</v>
+        <v>15.006954</v>
       </c>
       <c r="M195" t="n">
         <v>58</v>
@@ -10867,7 +10867,7 @@
         </is>
       </c>
       <c r="L196" s="3" t="n">
-        <v>0</v>
+        <v>14.180805</v>
       </c>
       <c r="M196" t="n">
         <v>58</v>
@@ -10920,7 +10920,7 @@
         </is>
       </c>
       <c r="L197" s="3" t="n">
-        <v>0</v>
+        <v>14.180805</v>
       </c>
       <c r="M197" t="n">
         <v>58</v>
@@ -10973,7 +10973,7 @@
         </is>
       </c>
       <c r="L198" s="3" t="n">
-        <v>0</v>
+        <v>14.180805</v>
       </c>
       <c r="M198" t="n">
         <v>58</v>
@@ -11026,7 +11026,7 @@
         </is>
       </c>
       <c r="L199" s="3" t="n">
-        <v>0</v>
+        <v>10.407774</v>
       </c>
       <c r="M199" t="n">
         <v>58</v>
@@ -11109,7 +11109,7 @@
         <v>4543.4</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>0</v>
+        <v>967.403445</v>
       </c>
     </row>
     <row r="3">
@@ -11128,7 +11128,7 @@
         <v>136.86</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>0</v>
+        <v>11.6563662</v>
       </c>
     </row>
     <row r="4">
@@ -11147,7 +11147,7 @@
         <v>55.54</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>0</v>
+        <v>11.8258545</v>
       </c>
     </row>
     <row r="5">
@@ -11166,7 +11166,7 @@
         <v>53.95</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>0</v>
+        <v>11.48730375</v>
       </c>
     </row>
     <row r="6">
@@ -11185,7 +11185,7 @@
         <v>1776.41</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>0</v>
+        <v>378.24209925</v>
       </c>
     </row>
     <row r="7">
@@ -11204,7 +11204,7 @@
         <v>1482.62</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0</v>
+        <v>126.2747454</v>
       </c>
     </row>
     <row r="8">
@@ -11223,7 +11223,7 @@
         <v>222.87</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>0</v>
+        <v>47.45459475</v>
       </c>
     </row>
     <row r="9">
@@ -11242,7 +11242,7 @@
         <v>121.13</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>0</v>
+        <v>25.79160525</v>
       </c>
     </row>
     <row r="10">
@@ -11261,7 +11261,7 @@
         <v>1706.98</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>0</v>
+        <v>145.3834866</v>
       </c>
     </row>
     <row r="11">
@@ -11280,7 +11280,7 @@
         <v>302.98</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>0</v>
+        <v>25.8048066</v>
       </c>
     </row>
     <row r="12">
@@ -11299,7 +11299,7 @@
         <v>355.16</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>0</v>
+        <v>30.2489772</v>
       </c>
     </row>
     <row r="13">
@@ -11318,7 +11318,7 @@
         <v>1099.26</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>0</v>
+        <v>93.62397420000001</v>
       </c>
     </row>
     <row r="14">
@@ -11337,7 +11337,7 @@
         <v>56.02</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>0</v>
+        <v>11.9280585</v>
       </c>
     </row>
     <row r="15">
@@ -11356,7 +11356,7 @@
         <v>139.18</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>0</v>
+        <v>29.6349015</v>
       </c>
     </row>
     <row r="16">
@@ -11375,7 +11375,7 @@
         <v>134.28</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>0</v>
+        <v>28.591569</v>
       </c>
     </row>
     <row r="17">
@@ -11394,7 +11394,7 @@
         <v>323.49</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>0</v>
+        <v>68.87910825</v>
       </c>
     </row>
     <row r="18">
@@ -11413,7 +11413,7 @@
         <v>51.81</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>0</v>
+        <v>11.03164425</v>
       </c>
     </row>
     <row r="19">
@@ -11432,7 +11432,7 @@
         <v>70.12</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>0</v>
+        <v>14.930301</v>
       </c>
     </row>
     <row r="20">
@@ -11451,7 +11451,7 @@
         <v>11.7</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>0</v>
+        <v>2.4912225</v>
       </c>
     </row>
     <row r="21">
@@ -11470,7 +11470,7 @@
         <v>2365.27</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>0</v>
+        <v>201.4500459</v>
       </c>
     </row>
     <row r="22">
@@ -11489,7 +11489,7 @@
         <v>697.6800000000001</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>0</v>
+        <v>148.553514</v>
       </c>
     </row>
     <row r="23">
@@ -11508,7 +11508,7 @@
         <v>437.09</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>0</v>
+        <v>93.06738825000001</v>
       </c>
     </row>
     <row r="24">
@@ -11527,7 +11527,7 @@
         <v>144.44</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>0</v>
+        <v>12.3019548</v>
       </c>
     </row>
     <row r="25">
@@ -11546,7 +11546,7 @@
         <v>159.53</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>0</v>
+        <v>33.96792525</v>
       </c>
     </row>
     <row r="26">
@@ -11565,7 +11565,7 @@
         <v>152.66</v>
       </c>
       <c r="E26" s="3" t="n">
-        <v>0</v>
+        <v>32.5051305</v>
       </c>
     </row>
     <row r="27">
@@ -11584,7 +11584,7 @@
         <v>230.8</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>0</v>
+        <v>49.14309</v>
       </c>
     </row>
     <row r="28">
@@ -11603,7 +11603,7 @@
         <v>88.38000000000001</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>0</v>
+        <v>18.8183115</v>
       </c>
     </row>
     <row r="29">
@@ -11622,7 +11622,7 @@
         <v>131.87</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>0</v>
+        <v>28.07841975</v>
       </c>
     </row>
     <row r="30">
@@ -11641,7 +11641,7 @@
         <v>43.42</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>0</v>
+        <v>9.245203500000001</v>
       </c>
     </row>
     <row r="31">
@@ -11660,7 +11660,7 @@
         <v>224.41</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>0</v>
+        <v>47.78249925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>